<commit_message>
Firmware split + last commit before RB3 bevel
</commit_message>
<xml_diff>
--- a/RB3/ClubRedTape/Full Combat BoM Template.xlsx
+++ b/RB3/ClubRedTape/Full Combat BoM Template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EdwardStuckey\Documents\GitHub\FightingRobot\RB3\ClubRedTape\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A54421B8-A951-42B8-9680-2C1BAC1A8D8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CBB3673-8502-4A7E-A49F-266D2C408952}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,6 +19,7 @@
     <sheet name="Electronics Calculations" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -121,7 +122,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="120">
   <si>
     <t>DO NOT ENTER VALUES FOR COLUMNS HIGHLIGHTED GREEN</t>
   </si>
@@ -463,9 +464,6 @@
     <t>Self Supplied</t>
   </si>
   <si>
-    <t>Plastic screws, club supplied</t>
-  </si>
-  <si>
     <t>X</t>
   </si>
   <si>
@@ -482,6 +480,12 @@
   </si>
   <si>
     <t>Robot disable switch</t>
+  </si>
+  <si>
+    <t>Plastic screws, club supplied (1/2 inch)</t>
+  </si>
+  <si>
+    <t>Plastic screws, club supplied (3/4 inch)</t>
   </si>
 </sst>
 </file>
@@ -1088,7 +1092,7 @@
   <dimension ref="A1:Q1007"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="108" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+      <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
@@ -1243,7 +1247,7 @@
         <v>7.99</v>
       </c>
       <c r="L4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="M4" s="2">
         <f t="shared" ref="M4:M15" si="0">IFERROR(K4/H4, 0)</f>
@@ -1286,7 +1290,7 @@
         <v>12.95</v>
       </c>
       <c r="L5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="M5" s="2">
         <f t="shared" si="0"/>
@@ -1434,7 +1438,7 @@
         <v>33</v>
       </c>
       <c r="D11" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="J11" s="9"/>
       <c r="K11" s="12">
@@ -1613,16 +1617,16 @@
     <row r="20" spans="1:15">
       <c r="A20" s="15"/>
       <c r="C20" t="s">
+        <v>118</v>
+      </c>
+      <c r="D20" t="s">
+        <v>114</v>
+      </c>
+      <c r="H20" t="s">
         <v>112</v>
       </c>
-      <c r="D20" t="s">
-        <v>115</v>
-      </c>
-      <c r="H20" t="s">
-        <v>113</v>
-      </c>
       <c r="I20">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="J20" t="s">
         <v>23</v>
@@ -1631,7 +1635,7 @@
         <v>0</v>
       </c>
       <c r="L20" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="M20" s="2">
         <f t="shared" si="3"/>
@@ -1649,6 +1653,18 @@
     <row r="21" spans="1:15">
       <c r="A21" s="15" t="s">
         <v>39</v>
+      </c>
+      <c r="C21" t="s">
+        <v>119</v>
+      </c>
+      <c r="H21" t="s">
+        <v>112</v>
+      </c>
+      <c r="I21">
+        <v>10</v>
+      </c>
+      <c r="J21" t="s">
+        <v>23</v>
       </c>
       <c r="K21" s="12">
         <v>0</v>

</xml_diff>